<commit_message>
was deleted spaces added json/xml write
</commit_message>
<xml_diff>
--- a/src/main/resources/statistics.xlsx
+++ b/src/main/resources/statistics.xlsx
@@ -29,16 +29,16 @@
     <t>University names</t>
   </si>
   <si>
+    <t>Fisica</t>
+  </si>
+  <si>
+    <t>[Московский Выдуманный Университет, Московский Придуманный Институт]</t>
+  </si>
+  <si>
     <t>Mедицина</t>
   </si>
   <si>
     <t>[Московский Государственный Медицинский Университет, Тамбовский Университет Медицины, Самарский Медицинский Институт]</t>
-  </si>
-  <si>
-    <t>Fisica</t>
-  </si>
-  <si>
-    <t>[Московский Выдуманный Университет, Московский Придуманный Институт]</t>
   </si>
 </sst>
 </file>
@@ -117,13 +117,13 @@
         <v>5</v>
       </c>
       <c r="B2" t="n" s="0">
-        <v>4.333333492279053</v>
+        <v>4.537499964237213</v>
       </c>
       <c r="C2" t="n" s="0">
-        <v>3.0</v>
+        <v>8.0</v>
       </c>
       <c r="D2" t="n" s="0">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="E2" t="s" s="0">
         <v>6</v>
@@ -134,13 +134,13 @@
         <v>7</v>
       </c>
       <c r="B3" t="n" s="0">
-        <v>4.537499964237213</v>
+        <v>4.333333492279053</v>
       </c>
       <c r="C3" t="n" s="0">
-        <v>8.0</v>
+        <v>3.0</v>
       </c>
       <c r="D3" t="n" s="0">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="E3" t="s" s="0">
         <v>8</v>

</xml_diff>